<commit_message>
in nhan phan kho
</commit_message>
<xml_diff>
--- a/GIAO DIEN PMQLTV.xlsx
+++ b/GIAO DIEN PMQLTV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WorkspaceProject\Web\Project_main\qltv.vlute.edu.vn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3937768-8F30-4F46-9E3E-6A3EBB455A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6702E272-DD5E-4C44-8997-296F7041F71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5235" windowWidth="29040" windowHeight="15720" xr2:uid="{2601CAB7-A912-4D99-BF3D-292060C84A98}"/>
   </bookViews>
@@ -307,7 +307,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +376,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -403,8 +411,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -417,18 +424,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -437,9 +444,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -457,11 +461,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -775,37 +778,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D32D401-AE19-4F1D-90AE-44C4E7CF1721}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="62.375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="29.875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="62.375" style="8" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
     <col min="4" max="4" width="96.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -816,8 +819,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -828,8 +831,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -840,8 +843,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -852,8 +855,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="11" t="s">
         <v>74</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -864,15 +867,15 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="11" t="s">
         <v>88</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -880,8 +883,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="11" t="s">
         <v>89</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -889,8 +892,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="11" t="s">
         <v>90</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -898,8 +901,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="11" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -907,15 +910,15 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -926,15 +929,15 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -944,9 +947,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -956,16 +959,16 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="12" t="s">
+    <row r="18" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -975,21 +978,21 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="12" t="s">
+    <row r="20" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="10" t="s">
         <v>80</v>
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="12"/>
+    <row r="21" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13"/>
+      <c r="B22" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -999,31 +1002,31 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
       <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="9" t="s">
+    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="13"/>
+      <c r="B24" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="4" t="s">
         <v>63</v>
       </c>
@@ -1039,34 +1042,30 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="6" t="s">
+    <row r="29" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
+    <row r="31" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
         <v>22</v>
       </c>
@@ -1077,7 +1076,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1087,8 +1086,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="2" t="s">
+    <row r="35" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D35" t="s">
@@ -1096,10 +1095,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="10"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="1" t="s">
         <v>28</v>
       </c>
@@ -1126,10 +1125,10 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="10"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="1" t="s">
         <v>33</v>
       </c>
@@ -1198,10 +1197,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="10"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="1" t="s">
         <v>48</v>
       </c>

</xml_diff>